<commit_message>
Scrum meeting notes and updated product backlog
</commit_message>
<xml_diff>
--- a/Product-Backlog/Product Backlog.xlsx
+++ b/Product-Backlog/Product Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Desktop/Industrial-Project-Team-9/Product-Backlog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Industrial-Project-Team-9/Product-Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84C62D1-6CB1-3F41-A9E0-EC3226FC414D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6835729C-F425-3B4E-BE7A-B233AC9378C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="27840" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="71">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>Oct 12th</t>
+  </si>
+  <si>
+    <t>Sprint 1-2</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -506,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -589,9 +595,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -608,6 +611,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -843,8 +852,8 @@
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="92" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -926,28 +935,29 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:19" ht="19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="38" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="8">
-        <f t="shared" ref="B3:B53" si="0">ROW()-2</f>
+        <f>ROW()-2</f>
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="9"/>
+      <c r="C3" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="E3" s="10"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="26">
-        <v>10</v>
-      </c>
-      <c r="I3" s="26">
-        <v>2</v>
-      </c>
-      <c r="J3" s="26">
-        <f>ROUND((H3/I3),J40)</f>
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>60</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>11</v>
@@ -961,28 +971,30 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" ht="19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="38" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>2</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="9"/>
+      <c r="C4" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
-      <c r="H4" s="26">
+      <c r="H4" s="27">
         <v>8</v>
       </c>
-      <c r="I4" s="26">
-        <v>3</v>
+      <c r="I4" s="27">
+        <v>2</v>
       </c>
       <c r="J4" s="26">
         <f>ROUND((H4/I4),0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K4" s="12" t="s">
         <v>11</v>
@@ -1001,25 +1013,27 @@
     <row r="5" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>3</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="9"/>
+      <c r="C5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>62</v>
+      </c>
       <c r="E5" s="10"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="26">
-        <v>10</v>
-      </c>
-      <c r="I5" s="26">
-        <v>1</v>
+      <c r="H5" s="27">
+        <v>9</v>
+      </c>
+      <c r="I5" s="27">
+        <v>4</v>
       </c>
       <c r="J5" s="26">
-        <f t="shared" ref="J5:J13" si="1">ROUND((H5/I5),0)</f>
-        <v>10</v>
+        <f>ROUND((H5/I5),0)</f>
+        <v>2</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>11</v>
@@ -1037,26 +1051,25 @@
     </row>
     <row r="6" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="9"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="26">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I6" s="26">
         <v>1</v>
       </c>
       <c r="J6" s="26">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f>ROUND((H6/I6),0)</f>
+        <v>6</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>11</v>
@@ -1075,24 +1088,27 @@
     <row r="7" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>5</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="9"/>
+      <c r="C7" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>62</v>
+      </c>
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="26">
+        <v>3</v>
+      </c>
+      <c r="I7" s="26">
         <v>1</v>
       </c>
-      <c r="I7" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>60</v>
+      <c r="J7" s="26">
+        <f>ROUND((H7/I7),0)</f>
+        <v>3</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>11</v>
@@ -1109,25 +1125,27 @@
     <row r="8" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>6</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="9"/>
+      <c r="C8" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="26">
+      <c r="H8" s="27">
+        <v>5</v>
+      </c>
+      <c r="I8" s="27">
         <v>3</v>
       </c>
-      <c r="I8" s="26">
-        <v>1</v>
-      </c>
       <c r="J8" s="26">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f>ROUND((H8/I8),0)</f>
+        <v>2</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>11</v>
@@ -1144,13 +1162,15 @@
     <row r="9" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>7</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="9"/>
+        <v>21</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
@@ -1158,11 +1178,11 @@
         <v>10</v>
       </c>
       <c r="I9" s="26">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J9" s="26">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f>ROUND((H9/I9),0)</f>
+        <v>3</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>11</v>
@@ -1179,13 +1199,15 @@
     <row r="10" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>8</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
@@ -1193,11 +1215,11 @@
         <v>10</v>
       </c>
       <c r="I10" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J10" s="26">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f>ROUND((H10/I10),J47)</f>
+        <v>5</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>11</v>
@@ -1214,24 +1236,27 @@
     <row r="11" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>9</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="27">
-        <v>1</v>
-      </c>
-      <c r="I11" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>60</v>
+      <c r="H11" s="26">
+        <v>8</v>
+      </c>
+      <c r="I11" s="26">
+        <v>3</v>
+      </c>
+      <c r="J11" s="26">
+        <f>ROUND((H11/I11),0)</f>
+        <v>3</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>11</v>
@@ -1248,25 +1273,27 @@
     <row r="12" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>10</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="9"/>
+      <c r="C12" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="26">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I12" s="26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J12" s="26">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>ROUND((H12/I12),0)</f>
+        <v>10</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>11</v>
@@ -1280,28 +1307,30 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" spans="1:19" ht="38" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="8">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="9"/>
+        <f>ROW()-2</f>
+        <v>11</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="27">
-        <v>8</v>
-      </c>
-      <c r="I13" s="27">
-        <v>2</v>
+      <c r="H13" s="26">
+        <v>9</v>
+      </c>
+      <c r="I13" s="26">
+        <v>1</v>
       </c>
       <c r="J13" s="26">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f>ROUND((H13/I13),0)</f>
+        <v>9</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>11</v>
@@ -1318,24 +1347,27 @@
     <row r="14" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>12</v>
       </c>
-      <c r="C14" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="9"/>
+      <c r="C14" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="27">
-        <v>1</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="27" t="s">
-        <v>60</v>
+      <c r="H14" s="26">
+        <v>10</v>
+      </c>
+      <c r="I14" s="26">
+        <v>5</v>
+      </c>
+      <c r="J14" s="26">
+        <f>ROUND((H14/I14),0)</f>
+        <v>2</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>11</v>
@@ -1349,27 +1381,30 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" spans="1:19" ht="19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="38" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>13</v>
       </c>
-      <c r="C15" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="9"/>
+      <c r="C15" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="27">
+      <c r="H15" s="26">
+        <v>7</v>
+      </c>
+      <c r="I15" s="26">
+        <v>5</v>
+      </c>
+      <c r="J15" s="26">
+        <f>ROUND((H15/I15),0)</f>
         <v>1</v>
-      </c>
-      <c r="I15" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="27" t="s">
-        <v>60</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>11</v>
@@ -1386,24 +1421,27 @@
     <row r="16" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>14</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="26">
-        <v>1</v>
-      </c>
-      <c r="I16" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>60</v>
+        <v>10</v>
+      </c>
+      <c r="I16" s="26">
+        <v>2</v>
+      </c>
+      <c r="J16" s="26">
+        <f>ROUND((H16/I16),0)</f>
+        <v>5</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>11</v>
@@ -1417,27 +1455,30 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="1:19" ht="38" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>15</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>63</v>
+      </c>
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="26">
-        <v>1</v>
-      </c>
-      <c r="I17" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="J17" s="26" t="s">
-        <v>60</v>
+      <c r="H17" s="27">
+        <v>7</v>
+      </c>
+      <c r="I17" s="27">
+        <v>3</v>
+      </c>
+      <c r="J17" s="26">
+        <f>ROUND((H17/I17),0)</f>
+        <v>2</v>
       </c>
       <c r="K17" s="12" t="s">
         <v>11</v>
@@ -1454,24 +1495,27 @@
     <row r="18" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>16</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>63</v>
+      </c>
       <c r="E18" s="10"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
-      <c r="H18" s="26">
-        <v>1</v>
-      </c>
-      <c r="I18" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="J18" s="26" t="s">
-        <v>60</v>
+      <c r="H18" s="27">
+        <v>10</v>
+      </c>
+      <c r="I18" s="27">
+        <v>2</v>
+      </c>
+      <c r="J18" s="26">
+        <f>ROUND((H18/I18),0)</f>
+        <v>5</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>11</v>
@@ -1485,28 +1529,30 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" spans="1:19" ht="19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="38" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>17</v>
       </c>
-      <c r="C19" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="19"/>
+      <c r="C19" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>63</v>
+      </c>
       <c r="E19" s="20"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
-      <c r="H19" s="26">
-        <v>10</v>
-      </c>
-      <c r="I19" s="26">
+      <c r="H19" s="27">
+        <v>9</v>
+      </c>
+      <c r="I19" s="27">
+        <v>4</v>
+      </c>
+      <c r="J19" s="26">
+        <f>ROUND((H19/I19),0)</f>
         <v>2</v>
-      </c>
-      <c r="J19" s="26">
-        <f t="shared" ref="J19:J37" si="2">ROUND((H19/I19),0)</f>
-        <v>5</v>
       </c>
       <c r="K19" s="12" t="s">
         <v>11</v>
@@ -1520,28 +1566,30 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
     </row>
-    <row r="20" spans="1:19" ht="38" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>18</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="12"/>
+        <v>39</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="E20" s="20"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="27">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I20" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J20" s="26">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>ROUND((H20/I20),0)</f>
+        <v>7</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>11</v>
@@ -1558,13 +1606,15 @@
     <row r="21" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>19</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="20"/>
+        <v>41</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="E21" s="20"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -1572,11 +1622,11 @@
         <v>9</v>
       </c>
       <c r="I21" s="27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J21" s="26">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f>ROUND((H21/I21),0)</f>
+        <v>9</v>
       </c>
       <c r="K21" s="12" t="s">
         <v>11</v>
@@ -1593,25 +1643,27 @@
     <row r="22" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>20</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="E22" s="20"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="27">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I22" s="27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J22" s="26">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f>ROUND((H22/I22),0)</f>
+        <v>10</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>11</v>
@@ -1625,16 +1677,18 @@
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
     </row>
-    <row r="23" spans="1:19" ht="19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="38" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>21</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="E23" s="20"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -1642,11 +1696,11 @@
         <v>10</v>
       </c>
       <c r="I23" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J23" s="26">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f>ROUND((H23/I23),0)</f>
+        <v>10</v>
       </c>
       <c r="K23" s="12" t="s">
         <v>11</v>
@@ -1660,25 +1714,30 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
-    <row r="24" spans="1:19" ht="19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="38" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="8"/>
+      <c r="B24" s="8">
+        <f>ROW()-2</f>
+        <v>22</v>
+      </c>
       <c r="C24" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E24" s="10"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="26">
-        <v>6</v>
-      </c>
-      <c r="I24" s="26">
+      <c r="H24" s="27">
+        <v>10</v>
+      </c>
+      <c r="I24" s="27">
         <v>1</v>
       </c>
       <c r="J24" s="26">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>ROUND((H24/I24),0)</f>
+        <v>10</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>11</v>
@@ -1695,25 +1754,27 @@
     <row r="25" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>23</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="20"/>
+        <v>46</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="E25" s="20"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
-      <c r="H25" s="26">
-        <v>3</v>
-      </c>
-      <c r="I25" s="26">
+      <c r="H25" s="27">
+        <v>9</v>
+      </c>
+      <c r="I25" s="27">
         <v>1</v>
       </c>
       <c r="J25" s="26">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f>ROUND((H25/I25),0)</f>
+        <v>9</v>
       </c>
       <c r="K25" s="12" t="s">
         <v>11</v>
@@ -1730,25 +1791,27 @@
     <row r="26" spans="1:19" ht="38" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>24</v>
       </c>
-      <c r="C26" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="9"/>
+      <c r="C26" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E26" s="10"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="27">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I26" s="27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J26" s="26">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f>ROUND((H26/I26),0)</f>
+        <v>3</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>11</v>
@@ -1765,25 +1828,27 @@
     <row r="27" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>25</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="9"/>
+      <c r="C27" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E27" s="10"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="27">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I27" s="27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J27" s="26">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>ROUND((H27/I27),0)</f>
+        <v>8</v>
       </c>
       <c r="K27" s="12" t="s">
         <v>11</v>
@@ -1797,28 +1862,32 @@
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
     </row>
-    <row r="28" spans="1:19" ht="19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="38" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>26</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="27">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I28" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J28" s="26">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <f>ROUND((H28/I28),0)</f>
+        <v>4</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>11</v>
@@ -1835,25 +1904,26 @@
     <row r="29" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>27</v>
       </c>
-      <c r="C29" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="9"/>
+      <c r="C29" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E29" s="25"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
-      <c r="H29" s="27">
-        <v>3</v>
-      </c>
-      <c r="I29" s="27">
-        <v>2</v>
-      </c>
-      <c r="J29" s="26">
-        <f t="shared" si="2"/>
-        <v>2</v>
+      <c r="H29" s="26">
+        <v>1</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="K29" s="12" t="s">
         <v>11</v>
@@ -1870,25 +1940,27 @@
     <row r="30" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>28</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="9"/>
+      <c r="C30" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E30" s="25"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
-      <c r="H30" s="27">
-        <v>9</v>
-      </c>
-      <c r="I30" s="27">
+      <c r="H30" s="26">
+        <v>3</v>
+      </c>
+      <c r="I30" s="26">
         <v>1</v>
       </c>
       <c r="J30" s="26">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <f>ROUND((H30/I30),0)</f>
+        <v>3</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>11</v>
@@ -1905,25 +1977,26 @@
     <row r="31" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>29</v>
       </c>
-      <c r="C31" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="9"/>
+      <c r="C31" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E31" s="25"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
       <c r="H31" s="27">
-        <v>10</v>
-      </c>
-      <c r="I31" s="27">
         <v>1</v>
       </c>
-      <c r="J31" s="26">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="I31" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="K31" s="12" t="s">
         <v>11</v>
@@ -1937,28 +2010,29 @@
       <c r="R31" s="18"/>
       <c r="S31" s="18"/>
     </row>
-    <row r="32" spans="1:19" ht="38" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>30</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E32" s="25"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
       <c r="H32" s="27">
-        <v>10</v>
-      </c>
-      <c r="I32" s="27">
         <v>1</v>
       </c>
-      <c r="J32" s="26">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="I32" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="K32" s="12" t="s">
         <v>11</v>
@@ -1975,25 +2049,26 @@
     <row r="33" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>31</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E33" s="25"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
       <c r="H33" s="27">
-        <v>5</v>
-      </c>
-      <c r="I33" s="27">
-        <v>3</v>
-      </c>
-      <c r="J33" s="26">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="I33" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="K33" s="12" t="s">
         <v>11</v>
@@ -2007,28 +2082,29 @@
       <c r="R33" s="18"/>
       <c r="S33" s="18"/>
     </row>
-    <row r="34" spans="1:19" ht="38" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>32</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="9"/>
+        <v>27</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E34" s="25"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
-      <c r="H34" s="27">
-        <v>10</v>
-      </c>
-      <c r="I34" s="27">
+      <c r="H34" s="26">
         <v>1</v>
       </c>
-      <c r="J34" s="26">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="I34" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="J34" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>11</v>
@@ -2042,28 +2118,29 @@
       <c r="R34" s="18"/>
       <c r="S34" s="18"/>
     </row>
-    <row r="35" spans="1:19" ht="19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="38" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>33</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E35" s="25"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
-      <c r="H35" s="27">
-        <v>9</v>
-      </c>
-      <c r="I35" s="27">
+      <c r="H35" s="26">
         <v>1</v>
       </c>
-      <c r="J35" s="26">
-        <f t="shared" si="2"/>
-        <v>9</v>
+      <c r="I35" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="J35" s="26" t="s">
+        <v>60</v>
       </c>
       <c r="K35" s="12" t="s">
         <v>11</v>
@@ -2077,28 +2154,30 @@
       <c r="R35" s="18"/>
       <c r="S35" s="18"/>
     </row>
-    <row r="36" spans="1:19" ht="38" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>34</v>
       </c>
-      <c r="C36" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="9"/>
+      <c r="C36" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E36" s="25"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="27">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I36" s="27">
         <v>3</v>
       </c>
       <c r="J36" s="26">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f>ROUND((H36/I36),0)</f>
+        <v>1</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>11</v>
@@ -2115,25 +2194,27 @@
     <row r="37" spans="1:19" ht="19" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="8">
-        <f t="shared" si="0"/>
+        <f>ROW()-2</f>
         <v>35</v>
       </c>
-      <c r="C37" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="9"/>
+      <c r="C37" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E37" s="25"/>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
       <c r="H37" s="27">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I37" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J37" s="26">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <f>ROUND((H37/I37),0)</f>
+        <v>2</v>
       </c>
       <c r="K37" s="12" t="s">
         <v>11</v>
@@ -2150,18 +2231,18 @@
     <row r="38" spans="1:19" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B38:B53" si="0">ROW()-2</f>
         <v>36</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="34"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33"/>
       <c r="L38" s="18"/>
       <c r="M38" s="17"/>
       <c r="N38" s="18"/>
@@ -2193,7 +2274,7 @@
         <v>8</v>
       </c>
       <c r="J39" s="26">
-        <f t="shared" ref="J39:J49" si="3">ROUND((H39/I39),0)</f>
+        <f t="shared" ref="J39:J49" si="1">ROUND((H39/I39),0)</f>
         <v>1</v>
       </c>
       <c r="K39" s="12" t="s">
@@ -2230,7 +2311,7 @@
         <v>3</v>
       </c>
       <c r="J40" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K40" s="12" t="s">
@@ -2267,7 +2348,7 @@
         <v>4</v>
       </c>
       <c r="J41" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K41" s="12" t="s">
@@ -2304,7 +2385,7 @@
         <v>2</v>
       </c>
       <c r="J42" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="K42" s="12" t="s">
@@ -2341,7 +2422,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="K43" s="12" t="s">
@@ -2378,7 +2459,7 @@
         <v>5</v>
       </c>
       <c r="J44" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K44" s="12" t="s">
@@ -2415,7 +2496,7 @@
         <v>1</v>
       </c>
       <c r="J45" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="K45" s="12" t="s">
@@ -2452,7 +2533,7 @@
         <v>2</v>
       </c>
       <c r="J46" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K46" s="12" t="s">
@@ -2495,7 +2576,7 @@
         <v>1</v>
       </c>
       <c r="J47" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="K47" s="12" t="s">
@@ -2538,7 +2619,7 @@
         <v>3</v>
       </c>
       <c r="J48" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K48" s="12" t="s">
@@ -2579,7 +2660,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K49" s="12" t="s">
@@ -3068,6 +3149,9 @@
       <c r="S71" s="4"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:K37">
+    <sortCondition descending="1" ref="D3:D37"/>
+  </sortState>
   <customSheetViews>
     <customSheetView guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>